<commit_message>
[documentation] filling in missing docstrings
</commit_message>
<xml_diff>
--- a/jupyter_prep/results_DecisionTree.xlsx
+++ b/jupyter_prep/results_DecisionTree.xlsx
@@ -530,10 +530,10 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.4047619047619048</v>
+        <v>0.4252026529108327</v>
       </c>
       <c r="C3">
-        <v>0.4041411042944785</v>
+        <v>0.4333458505444986</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
@@ -558,10 +558,10 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.5454257676479899</v>
+        <v>0.5649289099526066</v>
       </c>
       <c r="C5">
-        <v>0.5436188673292318</v>
+        <v>0.5635933806146571</v>
       </c>
       <c r="D5" t="s">
         <v>39</v>
@@ -572,10 +572,10 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.09417040358744394</v>
+        <v>0.1016597510373444</v>
       </c>
       <c r="C6">
-        <v>0.08069164265129683</v>
+        <v>0.09099350046425254</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
@@ -586,10 +586,10 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.06273062730627306</v>
+        <v>0.04330708661417323</v>
       </c>
       <c r="C7">
-        <v>0.0529595015576324</v>
+        <v>0.0352</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -600,10 +600,10 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.03053435114503817</v>
+        <v>0.02649006622516556</v>
       </c>
       <c r="C8">
-        <v>0.02359882005899705</v>
+        <v>0.02228412256267409</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
@@ -614,10 +614,10 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.03703703703703703</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>0.02790697674418605</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>39</v>
@@ -628,10 +628,10 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.04285714285714286</v>
+        <v>0.06179775280898876</v>
       </c>
       <c r="C10">
-        <v>0.02977667493796526</v>
+        <v>0.04988662131519275</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
@@ -642,10 +642,10 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0.09446254071661238</v>
+        <v>0.09508196721311475</v>
       </c>
       <c r="C11">
-        <v>0.07021791767554481</v>
+        <v>0.0703883495145631</v>
       </c>
       <c r="D11" t="s">
         <v>39</v>
@@ -656,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.158974358974359</v>
+        <v>0.157819225251076</v>
       </c>
       <c r="C12">
-        <v>0.1278350515463918</v>
+        <v>0.1403956604977664</v>
       </c>
       <c r="D12" t="s">
         <v>39</v>
@@ -670,10 +670,10 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0.1163265306122449</v>
+        <v>0.1062992125984252</v>
       </c>
       <c r="C13">
-        <v>0.09563758389261745</v>
+        <v>0.08925619834710743</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -684,10 +684,10 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="C14">
-        <v>0.02912621359223301</v>
+        <v>0.05825242718446601</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
@@ -698,10 +698,10 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>0.04672897196261682</v>
+        <v>0.02362204724409449</v>
       </c>
       <c r="C15">
-        <v>0.0352112676056338</v>
+        <v>0.01973684210526316</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
@@ -712,10 +712,10 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>0.02173913043478261</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>0.0144927536231884</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -726,10 +726,10 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>0.02395209580838323</v>
+        <v>0.05161290322580645</v>
       </c>
       <c r="C17">
-        <v>0.01918465227817746</v>
+        <v>0.03950617283950617</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -740,10 +740,10 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>0.07423580786026202</v>
+        <v>0.07906976744186046</v>
       </c>
       <c r="C18">
-        <v>0.06104129263913825</v>
+        <v>0.06261510128913443</v>
       </c>
       <c r="D18" t="s">
         <v>39</v>
@@ -754,10 +754,10 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>0.1878914405010438</v>
+        <v>0.1734390485629336</v>
       </c>
       <c r="C19">
-        <v>0.1868188894654904</v>
+        <v>0.1769464105156724</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -768,10 +768,10 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>0.07119741100323625</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="C20">
-        <v>0.05562579013906448</v>
+        <v>0.072992700729927</v>
       </c>
       <c r="D20" t="s">
         <v>39</v>
@@ -782,10 +782,10 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>0.07916666666666666</v>
+        <v>0.05990783410138249</v>
       </c>
       <c r="C21">
-        <v>0.06440677966101696</v>
+        <v>0.04585537918871253</v>
       </c>
       <c r="D21" t="s">
         <v>39</v>
@@ -796,10 +796,10 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>0.045</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="C22">
-        <v>0.04472049689440994</v>
+        <v>0.0472636815920398</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>
@@ -810,10 +810,10 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>0.05208333333333334</v>
+        <v>0.04081632653061224</v>
       </c>
       <c r="C23">
-        <v>0.04032258064516129</v>
+        <v>0.032</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
@@ -824,10 +824,10 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>0.04347826086956522</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>0.02898550724637681</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>39</v>
@@ -838,10 +838,10 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>0.01388888888888889</v>
+        <v>0.01639344262295082</v>
       </c>
       <c r="C25">
-        <v>0.01449275362318841</v>
+        <v>0.01574803149606299</v>
       </c>
       <c r="D25" t="s">
         <v>39</v>
@@ -880,10 +880,10 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>0.06481481481481481</v>
+        <v>0.0622568093385214</v>
       </c>
       <c r="C28">
-        <v>0.05233644859813084</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="D28" t="s">
         <v>39</v>
@@ -894,10 +894,10 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>0.4585714285714286</v>
+        <v>0.4440742503569728</v>
       </c>
       <c r="C29">
-        <v>0.4497898178421298</v>
+        <v>0.4356759280877889</v>
       </c>
       <c r="D29" t="s">
         <v>39</v>
@@ -908,10 +908,10 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>0.1741379310344827</v>
+        <v>0.1491228070175439</v>
       </c>
       <c r="C30">
-        <v>0.1640942323314379</v>
+        <v>0.1392301392301392</v>
       </c>
       <c r="D30" t="s">
         <v>39</v>
@@ -922,10 +922,10 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>0.2602739726027397</v>
+        <v>0.2335907335907336</v>
       </c>
       <c r="C31">
-        <v>0.2119521912350598</v>
+        <v>0.1917591125198098</v>
       </c>
       <c r="D31" t="s">
         <v>39</v>
@@ -936,10 +936,10 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>0.0196078431372549</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>0.0170940170940171</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
@@ -950,10 +950,10 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>0.308529945553539</v>
+        <v>0.3086876155268022</v>
       </c>
       <c r="C33">
-        <v>0.2687747035573123</v>
+        <v>0.2661354581673307</v>
       </c>
       <c r="D33" t="s">
         <v>39</v>
@@ -964,10 +964,10 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>0.02325581395348837</v>
+        <v>0.03260869565217391</v>
       </c>
       <c r="C34">
-        <v>0.01746724890829694</v>
+        <v>0.02553191489361702</v>
       </c>
       <c r="D34" t="s">
         <v>39</v>
@@ -978,10 +978,10 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>0.07291666666666667</v>
+        <v>0.07364341085271318</v>
       </c>
       <c r="C35">
-        <v>0.06140350877192983</v>
+        <v>0.0581039755351682</v>
       </c>
       <c r="D35" t="s">
         <v>39</v>
@@ -992,10 +992,10 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>0.3786539768864718</v>
+        <v>0.3824884792626728</v>
       </c>
       <c r="C36">
-        <v>0.3808547008547009</v>
+        <v>0.3908509922637067</v>
       </c>
       <c r="D36" t="s">
         <v>39</v>

</xml_diff>